<commit_message>
Revert "Eric ai buttons"
</commit_message>
<xml_diff>
--- a/documentation/project2_hours_team9.xlsx
+++ b/documentation/project2_hours_team9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Z\Desktop\Battleship Game Project 1 EECS448\eecs448-project-2\battleship\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landen/Desktop/Classes/Spring22/eecs448/Project2/battleship/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5352CD-9983-46B8-B388-5819ED346990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C68B28-66D0-EA43-8050-857CC579996F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE4D3226-987C-D248-9F68-E3A41E1223A4}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="17500" xr2:uid="{DE4D3226-987C-D248-9F68-E3A41E1223A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Hour Tracking - Project 2</t>
   </si>
@@ -55,9 +56,6 @@
   </si>
   <si>
     <t>Landen</t>
-  </si>
-  <si>
-    <t>Eric</t>
   </si>
 </sst>
 </file>
@@ -425,19 +423,19 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -448,7 +446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -459,7 +457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -470,24 +468,13 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44614</v>
-      </c>
-      <c r="C5">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C30">
         <f>SUM(C3:C29)</f>
-        <v>5</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>